<commit_message>
add interface & editing exp class
</commit_message>
<xml_diff>
--- a/projects/style_recognition/experiments.xlsx
+++ b/projects/style_recognition/experiments.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Experiment 1" sheetId="2" r:id="rId2"/>
     <sheet name="Experiment 2" sheetId="3" r:id="rId3"/>
     <sheet name="Experiment 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Experiment 4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="43">
   <si>
     <t>Project Name</t>
   </si>
@@ -32,6 +33,15 @@
   </si>
   <si>
     <t>Experiment Setup</t>
+  </si>
+  <si>
+    <t>Number of Classes: 2
+Input Length: 50
+Model Name: CharRNN
+Epochs: 10
+Batch Size: 128
+Device: cpu
+Notes: None</t>
   </si>
   <si>
     <t>Number of Classes: 2
@@ -64,7 +74,7 @@
     <t>STYLE_RECOGNITION</t>
   </si>
   <si>
-    <t>2018-12-15 23:42</t>
+    <t>2018-12-16 19:42</t>
   </si>
   <si>
     <t>Average Precision</t>
@@ -121,37 +131,40 @@
     <t>author: A.H. Al-Ghidani</t>
   </si>
   <si>
+    <t>date and time: 2018-12-16 19:41</t>
+  </si>
+  <si>
+    <t>172831</t>
+  </si>
+  <si>
+    <t>21603</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>CharRNN</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>cpu</t>
+  </si>
+  <si>
     <t>date and time: 2018-12-15 21:24</t>
   </si>
   <si>
-    <t>172831</t>
-  </si>
-  <si>
-    <t>21603</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>CharRNN</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
     <t>cuda</t>
   </si>
   <si>
     <t>date and time: 2018-12-13 15:37</t>
-  </si>
-  <si>
-    <t>cpu</t>
   </si>
   <si>
     <t>date and time: 2018-12-13 14:02</t>
@@ -294,6 +307,49 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1756422</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="learning_curve.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="381000"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -621,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -635,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -643,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -651,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -667,16 +723,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -684,16 +740,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>0.9838901711563193</v>
+        <v>0.622908760489604</v>
       </c>
       <c r="C6" s="1">
-        <v>0.9838047638543421</v>
+        <v>0.6053029262261299</v>
       </c>
       <c r="D6" s="1">
-        <v>0.9838191706837704</v>
+        <v>0.5882686849574266</v>
       </c>
       <c r="E6" s="1">
-        <v>0.984</v>
+        <v>0.602</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -701,16 +757,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>0.7667628997879563</v>
+        <v>0.9838901711563193</v>
       </c>
       <c r="C7" s="1">
-        <v>0.7187009967002718</v>
+        <v>0.9838047638543421</v>
       </c>
       <c r="D7" s="1">
-        <v>0.7061073616118854</v>
+        <v>0.9838191706837704</v>
       </c>
       <c r="E7" s="1">
-        <v>0.72</v>
+        <v>0.984</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -718,15 +774,32 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
+        <v>0.7667628997879563</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.7187009967002718</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.7061073616118854</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
         <v>0.9838985953537459</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>0.9839468478001268</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>0.9839118196087607</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>0.984</v>
       </c>
     </row>
@@ -751,47 +824,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -804,55 +877,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -865,26 +938,26 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>0.9838901711563193</v>
+        <v>0.622908760489604</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>0.9838047638543421</v>
+        <v>0.6053029262261299</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1">
-        <v>0.9838191706837704</v>
+        <v>0.5882686849574266</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -917,47 +990,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -970,55 +1043,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1031,26 +1104,26 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>0.7667628997879563</v>
+        <v>0.9838901711563193</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>0.7187009967002718</v>
+        <v>0.9838047638543421</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1">
-        <v>0.7061073616118854</v>
+        <v>0.9838191706837704</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1083,47 +1156,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1136,55 +1209,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1197,7 +1270,173 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.7667628997879563</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.7187009967002718</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.7061073616118854</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="26" width="30.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B16" s="1">
         <v>0.9838985953537459</v>
@@ -1205,7 +1444,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
         <v>0.9839468478001268</v>
@@ -1213,7 +1452,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1">
         <v>0.9839118196087607</v>

</xml_diff>

<commit_message>
a lot of modifications! :D
</commit_message>
<xml_diff>
--- a/projects/style_recognition/experiments.xlsx
+++ b/projects/style_recognition/experiments.xlsx
@@ -12,13 +12,15 @@
     <sheet name="Experiment 2" sheetId="3" r:id="rId3"/>
     <sheet name="Experiment 3" sheetId="4" r:id="rId4"/>
     <sheet name="Experiment 4" sheetId="5" r:id="rId5"/>
+    <sheet name="Experiment 5" sheetId="6" r:id="rId6"/>
+    <sheet name="Experiment 6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="48">
   <si>
     <t>Project Name</t>
   </si>
@@ -56,10 +58,28 @@
     <t>Number of Classes: 2
 Input Length: 50
 Model Name: CharRNN
+Epochs: 8
+Batch Size: 128
+Device: cpu
+Notes: None</t>
+  </si>
+  <si>
+    <t>Number of Classes: 2
+Input Length: 50
+Model Name: CharRNN
 Epochs: 2
 Batch Size: 128
 Device: cpu
 Notes: None</t>
+  </si>
+  <si>
+    <t>Number of Classes: 2
+Input Length: 50
+Model Name: CharRNN
+Epochs: 10
+Batch Size: 128
+Device: cuda
+Notes: _new</t>
   </si>
   <si>
     <t>Number of Classes: 2
@@ -74,7 +94,7 @@
     <t>STYLE_RECOGNITION</t>
   </si>
   <si>
-    <t>2018-12-16 19:42</t>
+    <t>2018-12-16 23:13</t>
   </si>
   <si>
     <t>Average Precision</t>
@@ -164,7 +184,16 @@
     <t>cuda</t>
   </si>
   <si>
+    <t>date and time: 2018-12-16 23:13</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>date and time: 2018-12-13 15:37</t>
+  </si>
+  <si>
+    <t>date and time: 2018-12-16 18:53</t>
   </si>
   <si>
     <t>date and time: 2018-12-13 14:02</t>
@@ -350,6 +379,92 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1756422</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="learning_curve.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="381000"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1756422</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="learning_curve.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="381000"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -677,7 +792,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -691,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -699,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -707,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -723,16 +838,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -774,16 +889,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>0.7667628997879563</v>
+        <v>0.5983721262316151</v>
       </c>
       <c r="C8" s="1">
-        <v>0.7187009967002718</v>
+        <v>0.5935014522652624</v>
       </c>
       <c r="D8" s="1">
-        <v>0.7061073616118854</v>
+        <v>0.58994708994709</v>
       </c>
       <c r="E8" s="1">
-        <v>0.72</v>
+        <v>0.596</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -791,15 +906,49 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
+        <v>0.7667628997879563</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.7187009967002718</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.7061073616118854</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.9857832861265355</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.985780844414788</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.9857618332241506</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
         <v>0.9838985953537459</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>0.9839468478001268</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D11" s="1">
         <v>0.9839118196087607</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E11" s="1">
         <v>0.984</v>
       </c>
     </row>
@@ -824,47 +973,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -877,55 +1026,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -938,7 +1087,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>0.622908760489604</v>
@@ -946,7 +1095,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>0.6053029262261299</v>
@@ -954,7 +1103,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>0.5882686849574266</v>
@@ -990,47 +1139,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1043,55 +1192,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1104,7 +1253,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>0.9838901711563193</v>
@@ -1112,7 +1261,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>0.9838047638543421</v>
@@ -1120,7 +1269,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>0.9838191706837704</v>
@@ -1156,47 +1305,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1209,55 +1358,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1270,26 +1419,26 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
-        <v>0.7667628997879563</v>
+        <v>0.5983721262316151</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
-        <v>0.7187009967002718</v>
+        <v>0.5935014522652624</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
-        <v>0.7061073616118854</v>
+        <v>0.58994708994709</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1322,47 +1471,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1375,47 +1524,47 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>39</v>
@@ -1423,7 +1572,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1436,7 +1585,339 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.7667628997879563</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.7187009967002718</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.7061073616118854</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="26" width="30.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.9857832861265355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.985780844414788</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.9857618332241506</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="26" width="30.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>0.9838985953537459</v>
@@ -1444,7 +1925,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>0.9839468478001268</v>
@@ -1452,7 +1933,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>0.9839118196087607</v>

</xml_diff>

<commit_message>
fixing loading model bug
</commit_message>
<xml_diff>
--- a/projects/style_recognition/experiments.xlsx
+++ b/projects/style_recognition/experiments.xlsx
@@ -14,13 +14,14 @@
     <sheet name="Experiment 4" sheetId="5" r:id="rId5"/>
     <sheet name="Experiment 5" sheetId="6" r:id="rId6"/>
     <sheet name="Experiment 6" sheetId="7" r:id="rId7"/>
+    <sheet name="Experiment 7" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="51">
   <si>
     <t>Project Name</t>
   </si>
@@ -85,6 +86,15 @@
     <t>Number of Classes: 2
 Input Length: 50
 Model Name: CharRNN
+Epochs: 3
+Batch Size: 128
+Device: cuda
+Notes: None</t>
+  </si>
+  <si>
+    <t>Number of Classes: 2
+Input Length: 50
+Model Name: CharRNN
 Epochs: 5
 Batch Size: 128
 Device: cuda
@@ -94,7 +104,7 @@
     <t>STYLE_RECOGNITION</t>
   </si>
   <si>
-    <t>2018-12-16 23:13</t>
+    <t>2018-12-17 01:42</t>
   </si>
   <si>
     <t>Average Precision</t>
@@ -194,6 +204,12 @@
   </si>
   <si>
     <t>date and time: 2018-12-16 18:53</t>
+  </si>
+  <si>
+    <t>date and time: 2018-12-16 23:25</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>date and time: 2018-12-13 14:02</t>
@@ -465,6 +481,49 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1756422</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="learning_curve.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="381000"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -792,7 +851,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -806,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -814,7 +873,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -822,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -838,16 +897,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -940,15 +999,32 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
+        <v>0.9816321265188687</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.9816731162480927</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.9816462742162386</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
         <v>0.9838985953537459</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>0.9839468478001268</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>0.9839118196087607</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>0.984</v>
       </c>
     </row>
@@ -973,47 +1049,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1026,55 +1102,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1087,7 +1163,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>0.622908760489604</v>
@@ -1095,7 +1171,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>0.6053029262261299</v>
@@ -1103,7 +1179,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0.5882686849574266</v>
@@ -1139,47 +1215,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1192,55 +1268,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1253,7 +1329,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>0.9838901711563193</v>
@@ -1261,7 +1337,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>0.9838047638543421</v>
@@ -1269,7 +1345,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0.9838191706837704</v>
@@ -1305,47 +1381,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1358,55 +1434,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1419,7 +1495,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>0.5983721262316151</v>
@@ -1427,7 +1503,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>0.5935014522652624</v>
@@ -1435,7 +1511,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0.58994708994709</v>
@@ -1471,47 +1547,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1524,55 +1600,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1585,7 +1661,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>0.7667628997879563</v>
@@ -1593,7 +1669,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>0.7187009967002718</v>
@@ -1601,7 +1677,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0.7061073616118854</v>
@@ -1637,47 +1713,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1690,55 +1766,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1751,7 +1827,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>0.9857832861265355</v>
@@ -1759,7 +1835,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>0.985780844414788</v>
@@ -1767,7 +1843,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0.9857618332241506</v>
@@ -1803,47 +1879,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1856,55 +1932,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1917,7 +1993,173 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.9816321265188687</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.9816731162480927</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.9816462742162386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="26" width="30.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>0.9838985953537459</v>
@@ -1925,7 +2167,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>0.9839468478001268</v>
@@ -1933,7 +2175,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0.9839118196087607</v>

</xml_diff>